<commit_message>
algunos cambios en los datos de TC-Crredito Forzado
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDITO FORZADO- Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDITO FORZADO- Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B5CA63-3554-4E7C-BDB0-8D56C5ACB8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FC5E09-E066-43DB-8524-60AA89562ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CREDITO FORZADO" sheetId="10" r:id="rId1"/>
@@ -26,12 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -425,12 +422,6 @@
     <t>"operacion":{"vendedor":{"cuit":"20000001644","cbu":"0000492700000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion5"},"comprador":{"cuit":"20000001644","cuenta":{"cbu":"0000492700000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001644","cuenta":{"cbu":"0000492700000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001644","cuenta":{"cbu":"9980000400000000000659"}}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001652","cbu":"0000494100000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion6"},"comprador":{"cuit":"20000001652","cuenta":{"cbu":"0000494100000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001652","cuenta":{"cbu":"0000494100000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001652","cuenta":{"cbu":"0440000400000000000703"}}}}|"id":"debin.id","aviso":"all","endpoint":"RecCVU04","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001555","cbu":"0000495800000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion7"},"comprador":{"cuit":"20000001555","cuenta":{"cbu":"0000495800000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001555","cuenta":{"cbu":"0000495800000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001660","cuenta":{"cbu":"0440000400000000000710"}}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
     <t>"operacion":{"vendedor":{"cuit":"20000001679","cbu":"0000493400000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion8"},"comprador":{"cuit":"20000001679","cuenta":{"cbu":"0000493400000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001679","cuenta":{"cbu":"0000493400000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001679","cuenta":{"cbu":"9980000400000000000710"}}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
   </si>
   <si>
@@ -446,15 +437,9 @@
     <t>"operacion":{"vendedor":{"cuit":"20000001628","cbu":"0000487300000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion3"},"comprador":{"cuit":"20000001628","cuenta":{"cbu":"0000487300000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001628","cuenta":{"cbu":"0000487300000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001628","cuenta":{"cbu":"9980000400000000000611"}}}}|"operacionOriginal":{"detalle":{"importe":10}},"comprador":{"cuit":"20000001628","cuenta":{"cbu":"0000487300000000000017"}},"vendedor":{"cuit":"20000001628","cuenta":{"cbu":"0000487300000000000000"}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001717","cbu":"0000486600000000000000","banco":"000","sucursal":"0486"},"comprador":{"cuenta":{"cbu":"0000486600000000000017"},"cuit":"20000001717"},"detalle":{"importe":1000,"id_billetera":486}}}|"operacion":{"comprador":{"cuit":"20000001717","cuenta":{"cbu":"9980000400000000000796"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
     <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 403 - Debin QR Coelsa Coelsa - OK</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001725","cbu":"0000484200000000000000","banco":"000","sucursal":"0484"},"comprador":{"cuenta":{"cbu":"0000484200000000000017"},"cuit":"20000001725"},"detalle":{"importe":1000,"id_billetera":484}}}|"operacion":{"comprador":{"cuit":"20000001725","cuenta":{"cbu":"9980000400000000000819"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
     <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 404 - Debin QR Coelsa Coelsa - OK</t>
   </si>
   <si>
@@ -516,6 +501,18 @@
   </si>
   <si>
     <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 00: Crédito realizado - Contracargo QR Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001725","cbu":"0000484200000000000000","banco":"000","sucursal":"0484"},"comprador":{"cuenta":{"cbu":"0000484200000000000017"},"cuit":"20000001725"},"detalle":{"importe":10,"id_billetera":484}}}|"operacion":{"comprador":{"cuit":"20000001725","cuenta":{"cbu":"9980000400000000000819"}},"detalle":{"importe":10}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001717","cbu":"0000486600000000000000","banco":"000","sucursal":"0486"},"comprador":{"cuenta":{"cbu":"0000486600000000000017"},"cuit":"20000001717"},"detalle":{"importe":10,"id_billetera":486}}}|"operacion":{"comprador":{"cuit":"20000001717","cuenta":{"cbu":"9980000400000000000796"}},"detalle":{"importe":10}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001652","cbu":"0000494100000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion6"},"comprador":{"cuit":"20000001652","cuenta":{"cbu":"0000494100000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001652","cuenta":{"cbu":"0000494100000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001652","cuenta":{"cbu":"9980000400000000000673"}}}}|"id":"debin.id","aviso":"all","endpoint":"RecCVU04","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001555","cbu":"0000495800000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion7"},"comprador":{"cuit":"20000001555","cuenta":{"cbu":"0000495800000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001555","cuenta":{"cbu":"0000495800000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001660","cuenta":{"cbu":"9980000400000000000697"}}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
   </si>
 </sst>
 </file>
@@ -870,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC0A671-2C0C-430F-865C-9634A4BA3E48}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +963,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>61224</v>
       </c>
@@ -987,7 +984,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>61228</v>
       </c>
@@ -1008,7 +1005,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>61229</v>
       </c>
@@ -1029,7 +1026,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>61225</v>
       </c>
@@ -1040,7 +1037,7 @@
         <v>72</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f t="shared" ref="D6:D10" si="0">_xlfn.CONCAT(G$4,F8,H$4,F8,I$4,F8,J$4)</f>
+        <f t="shared" ref="D8:D10" si="0">_xlfn.CONCAT(G$4,F8,H$4,F8,I$4,F8,J$4)</f>
         <v>{"StatusCode":200,"Mensaje":{"avisos":[{"endpoint":"CashOut03","accion":"AvisoCashOutPendiente","send":{"respuesta":{"codigo":"7600"}},"statusCode":"200"},{"endpoint":"CashOut03","accion":"Credito","send":{"Respuesta":{"codigo":"03"}},"statusCode":"200"}]}}</v>
       </c>
       <c r="E8" t="s">
@@ -1050,7 +1047,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>61226</v>
       </c>
@@ -1639,7 +1636,7 @@
         <v>9</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9" t="s">
@@ -1654,7 +1651,7 @@
         <v>9</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9" t="s">
@@ -1669,7 +1666,7 @@
         <v>9</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9" t="s">
@@ -1684,7 +1681,7 @@
         <v>9</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9" t="s">
@@ -1699,7 +1696,7 @@
         <v>11</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9" t="s">
@@ -1714,7 +1711,7 @@
         <v>11</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9" t="s">
@@ -1729,7 +1726,7 @@
         <v>11</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9" t="s">
@@ -1744,11 +1741,11 @@
         <v>10</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1759,11 +1756,11 @@
         <v>10</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1774,11 +1771,11 @@
         <v>10</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1789,11 +1786,11 @@
         <v>10</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1804,11 +1801,11 @@
         <v>10</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1819,11 +1816,11 @@
         <v>10</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1834,11 +1831,11 @@
         <v>10</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1849,11 +1846,11 @@
         <v>10</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1864,11 +1861,11 @@
         <v>10</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1879,11 +1876,11 @@
         <v>13</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1894,11 +1891,11 @@
         <v>13</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1909,11 +1906,11 @@
         <v>13</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mas cambios de credito forzado para QA
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDITO FORZADO- Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDITO FORZADO- Escenarios y Casos de Pruebas.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C23A20A-90D7-44A7-B164-334C8E2A7208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBCCCA5-16F4-4595-8C26-15AB17D080EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CREDITO FORZADO" sheetId="10" r:id="rId1"/>
-    <sheet name="CREDITO FORZADO HP" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CREDITO FORZADO'!$A$1:$E$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CREDITO FORZADO HP'!$A$1:$E$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="162">
   <si>
     <t>Parametros</t>
   </si>
@@ -68,15 +66,9 @@
     <t>Debin*-&gt;ConfirmaDebitoCVU*-&gt;ConfirmaDebito*-&gt;aviso*</t>
   </si>
   <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Debin QR Coelsa Coelsa - OK</t>
-  </si>
-  <si>
     <t>QRDebin*-&gt;ConfirmaDebito*-&gt;aviso*</t>
   </si>
   <si>
-    <t>Credito Forzado - Agregado a broker/push - DebinQR Coelsa Billetera - OK</t>
-  </si>
-  <si>
     <t>Debin*-&gt;ConfirmaDebitoCVU*-&gt;ConfirmaDebito*-&gt;ContraCargo*-&gt;aviso*</t>
   </si>
   <si>
@@ -86,15 +78,6 @@
     <t>QRDebin*-&gt;ConfirmaDebito*-&gt;QRSolicitudContraCargo*-&gt;aviso*</t>
   </si>
   <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Contracargo QR Coelsa Coelsa - OK</t>
-  </si>
-  <si>
-    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - Refund QR Coelsa Billetera - OK</t>
-  </si>
-  <si>
-    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;RefundValidation-&gt;Refund-&gt;aviso*</t>
-  </si>
-  <si>
     <t>Credito Forzado - Agregado a broker/push -CVU-CVU- AvisoCredito responde un 200 con codigo 00: Credito realizado - Debin Recurrente - OK</t>
   </si>
   <si>
@@ -107,18 +90,6 @@
     <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con codigo 00: Credito realizado - TRX ISO - OK</t>
   </si>
   <si>
-    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"detalle":{"importe":1000}}}|"operacion_original":{"detalle":{"importe":250}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
     <t>CreditoISO*-&gt;aviso*</t>
   </si>
   <si>
@@ -426,13 +397,136 @@
   </si>
   <si>
     <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000000796","cbu":"0000230300000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion21"},"comprador":{"cuit":"20000000796","cuenta":{"cbu":"0000230300000000000017"}}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000796","cuenta":{"cbu":"0000230300000000000017"}}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000761","cuenta":{"cbu":"0440000400000000000772"}}}}|"banco":"044","operacionOriginal":{"detalle":{"importe":10}},"comprador":{"cuit":"20000000796","cuenta":{"cbu":"0000230300000000000017"}},"vendedor":{"cuit":"20000000796","cuenta":{"cbu":"0000230300000000000000"}}}|"id":"debin.id","aviso":"all","endpoint":"ContRec404","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000000818","cbu":"0000231000000000000000","banco":"000","sucursal":"0231"},"comprador":{"cuenta":{"cbu":"0000231000000000000017"},"cuit":"20000000818"},"detalle":{"importe":1000,"id_billetera":231}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000818","cuenta":{"cbu":"0440000400000000000796"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 403 - Debin QR Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001016","cbu":"0000232700000000000000","banco":"000","sucursal":"0232"},"comprador":{"cuenta":{"cbu":"0000232700000000000017"},"cuit":"20000001016"},"detalle":{"importe":1000,"id_billetera":177}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000826","cuenta":{"cbu":"0440000400000000000819"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 404 - Debin QR Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001024","cbu":"0000233400000000000000","banco":"000","sucursal":"0233"},"comprador":{"cuenta":{"cbu":"0000233400000000000017"},"cuit":"20000001024"},"detalle":{"importe":1000,"id_billetera":233}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000834","cuenta":{"cbu":"0440000400000000000833"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 00: Crédito realizado - Debin QR Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001083","cbu":"0000238900000000000000","banco":"000","sucursal":"0238"},"comprador":{"cuenta":{"cbu":"0000238900000000000017"},"cuit":"20000001083"},"detalle":{"importe":1000,"id_billetera":238}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000893","cuenta":{"cbu":"0440000400000000000956"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 07: Acreditación pendiente (EN SCREENING) - Debin QR Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001040","cbu":"0000235800000000000000","banco":"000","sucursal":"0235"},"comprador":{"cuenta":{"cbu":"0000235800000000000017"},"cuit":"20000001040"},"detalle":{"importe":1000,"id_billetera":235}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000850","cuenta":{"cbu":"0440000400000000000871"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 03: Cuenta inexistente - Debin QR Coelsa Coelsa</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001059","cbu":"'0000236500000000000000","banco":"000","sucursal":"0236"},"comprador":{"cuenta":{"cbu":"0000236500000000000017"},"cuit":"20000001059"},"detalle":{"importe":1000,"id_billetera":236}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000869","cuenta":{"cbu":"0440000400000000000895"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 04: Cuenta no habilitada - Debin QR Coelsa Coelsa</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001075","cbu":"0000237200000000000000","banco":"000","sucursal":"0237"},"comprador":{"cuenta":{"cbu":"0000237200000000000017"},"cuit":"20000001075"},"detalle":{"importe":1000,"id_billetera":237}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000885","cuenta":{"cbu":"0440000400000000000932"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 06: Scoring Alto - Debin QR Coelsa Coelsa</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001032","cbu":"0000234100000000000000","banco":"000","sucursal":"0234"},"comprador":{"cuenta":{"cbu":"0000234100000000000017"},"cuit":"20000001032"},"detalle":{"importe":1000,"id_billetera":234}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000842","cuenta":{"cbu":"0440000400000000000857"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 02: Datos incorrectos - Debin QR Coelsa Coelsa - OK </t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001067","cbu":"0000126300000000000000","banco":"000","sucursal":"0126"},"comprador":{"cuenta":{"cbu":"0000126300000000000017"},"cuit":"20000001067"},"detalle":{"importe":1000,"id_billetera":126}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000877","cuenta":{"cbu":"0440000400000000000918"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 05: Error interno - Debin QR Coelsa Coelsa - OK </t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000000818","cbu":"0000231000000000000000","banco":"000","sucursal":"0231"},"comprador":{"cuenta":{"cbu":"0000231000000000000017"},"cuit":"20000000818"},"detalle":{"importe":1000,"id_billetera":231}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000818","cuenta":{"cbu":"0440000400000000000796"}},"detalle":{"importe":1000}}}|"banco":"044","operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20000000818","cbu":"0000231000000000000000"}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 403 - Contracargo QR Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001016","cbu":"0000232700000000000000","banco":"000","sucursal":"0232"},"comprador":{"cuenta":{"cbu":"0000232700000000000017"},"cuit":"20000001016"},"detalle":{"importe":1000,"id_billetera":177}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000826","cuenta":{"cbu":"0440000400000000000819"}},"detalle":{"importe":1000}}}|"banco":"044","operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20000001016","cbu":"0000232700000000000000"}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 404 - Contracargo QR Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001024","cbu":"0000233400000000000000","banco":"000","sucursal":"0233"},"comprador":{"cuenta":{"cbu":"0000233400000000000017"},"cuit":"20000001024"},"detalle":{"importe":1000,"id_billetera":233}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000834","cuenta":{"cbu":"0440000400000000000833"}},"detalle":{"importe":1000}}}|"banco":"044","operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20000001024","cbu":"0000233400000000000000"}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 00: Crédito realizado - Contracargo QR Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>PaymentValidation*-&gt;Payment*-&gt;QRSolicitudContraCargoPayment*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>"banco":"902"|"banco":"902"|"banco":"016","operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 00: Crédito realizado - Contracargo QR Coelsa Aceptador - OK</t>
+  </si>
+  <si>
+    <t>PaymentValidation*-&gt;Payment*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>"banco":"902"|"banco":"902"|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 00: Crédito realizado - Coelsa Aceptador - OK</t>
+  </si>
+  <si>
+    <t>CREDIN - Modificación Control Garantías - Llamada Crédito/Débito - Caso OK</t>
+  </si>
+  <si>
+    <t>se debe crear comprador para otro banco</t>
+  </si>
+  <si>
+    <t>CREDIN - Modificación Control Garantías - Avisos con codigos correctos - ERROR 0120 en Garantias -&gt; 0510 FONDOS INSUF.</t>
+  </si>
+  <si>
+    <t>Recurrente CVU-CVU - Modificación Control Garantías - Llamada Crédito/Débito - Caso OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar la operación con un importe mayor a las garantías del banco débito y dar de alta un comprador en otro banco </t>
+  </si>
+  <si>
+    <t>Recurrente CVU-CVU - Modificación Control Garantías - Avisos con codigos correctos - ERROR 0120 en Garantias -&gt; 0510 FONDOS INSUF.</t>
+  </si>
+  <si>
+    <t>Debin Spot CBU-CBU - Modificación Control Garantías - Llamada Crédito/Débito - Caso OK</t>
+  </si>
+  <si>
+    <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000000419","cbu":"0000219800000000000000","banco":"000","recurrencia":true},"comprador":{"cuit":"20000000419","cuenta":{"cbu":"0000219800000000000017"}}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000346","cuenta":{"cbu":"0440218500000000000437"}}}}|"id":"debin.id","aviso":"all","endpoint":"SpotCVUHP","producto":"responder"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dar de alta cbu para vendedor y comprador en distintos bancos </t>
+  </si>
+  <si>
+    <t>Debin Spot CBU-CBU - Modificación Control Garantías - Avisos con codigos correctos - ERROR 0120 en Garantias -&gt; 0510 FONDOS INSUF.</t>
+  </si>
+  <si>
+    <t>CASHOUT - Modificación Control Garantías - Llamada Crédito/Débito - Caso OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,6 +540,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -456,7 +556,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -492,13 +592,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC0A671-2C0C-430F-865C-9634A4BA3E48}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="D73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,11 +926,11 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -835,11 +941,11 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -850,7 +956,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
@@ -865,10 +971,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -879,10 +985,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -893,10 +999,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -907,10 +1013,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -921,10 +1027,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -935,10 +1041,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -949,11 +1055,11 @@
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="10" t="s">
-        <v>30</v>
+      <c r="E11" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -964,11 +1070,11 @@
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="10" t="s">
-        <v>31</v>
+      <c r="E12" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -979,10 +1085,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -994,10 +1100,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1008,10 +1114,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1022,10 +1128,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1036,10 +1142,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1050,10 +1156,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1064,10 +1170,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1075,14 +1181,14 @@
         <v>61432</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="10" t="s">
-        <v>79</v>
+      <c r="E20" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1090,14 +1196,14 @@
         <v>61433</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="10" t="s">
-        <v>80</v>
+      <c r="E21" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1105,14 +1211,14 @@
         <v>61435</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1120,13 +1226,13 @@
         <v>61436</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1134,13 +1240,13 @@
         <v>61440</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1148,13 +1254,13 @@
         <v>61441</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1165,11 +1271,11 @@
         <v>9</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="10" t="s">
-        <v>90</v>
+      <c r="E26" s="8" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1180,11 +1286,11 @@
         <v>9</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="10" t="s">
-        <v>91</v>
+      <c r="E27" s="8" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1195,10 +1301,10 @@
         <v>9</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E28" s="10" t="s">
         <v>92</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1209,10 +1315,10 @@
         <v>9</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E29" s="10" t="s">
         <v>93</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1223,10 +1329,10 @@
         <v>9</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" s="10" t="s">
         <v>94</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1237,10 +1343,10 @@
         <v>9</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" s="10" t="s">
         <v>95</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1251,10 +1357,10 @@
         <v>9</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1265,10 +1371,10 @@
         <v>9</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1279,10 +1385,10 @@
         <v>9</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1290,14 +1396,14 @@
         <v>61320</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D35" s="4"/>
-      <c r="E35" s="10" t="s">
-        <v>35</v>
+      <c r="E35" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1305,14 +1411,14 @@
         <v>61321</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="10" t="s">
-        <v>36</v>
+      <c r="E36" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1320,13 +1426,13 @@
         <v>61323</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>20</v>
+        <v>37</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1334,13 +1440,13 @@
         <v>61324</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1348,13 +1454,13 @@
         <v>61328</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1362,13 +1468,13 @@
         <v>61329</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1376,13 +1482,13 @@
         <v>61325</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1390,13 +1496,13 @@
         <v>61326</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1404,13 +1510,13 @@
         <v>61327</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>64</v>
+        <v>69</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1421,11 +1527,11 @@
         <v>9</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D44" s="4"/>
-      <c r="E44" s="10" t="s">
-        <v>110</v>
+      <c r="E44" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1436,11 +1542,11 @@
         <v>9</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D45" s="4"/>
-      <c r="E45" s="10" t="s">
-        <v>111</v>
+      <c r="E45" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1451,10 +1557,10 @@
         <v>9</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>19</v>
+        <v>111</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1465,10 +1571,10 @@
         <v>9</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E47" s="10" t="s">
         <v>112</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1479,10 +1585,10 @@
         <v>9</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E48" s="10" t="s">
         <v>113</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1493,10 +1599,10 @@
         <v>9</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E49" s="10" t="s">
         <v>114</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1507,10 +1613,10 @@
         <v>9</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E50" s="10" t="s">
         <v>115</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1521,10 +1627,10 @@
         <v>9</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E51" s="10" t="s">
         <v>116</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1535,10 +1641,10 @@
         <v>9</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E52" s="10" t="s">
         <v>117</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -1546,13 +1652,13 @@
         <v>61209</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>108</v>
+        <v>119</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -1560,13 +1666,13 @@
         <v>61210</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>109</v>
+        <v>120</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -1574,113 +1680,336 @@
         <v>61212</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="9">
+        <v>61187</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
+        <v>61188</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A58" s="9">
+        <v>61190</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>61191</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A60" s="9">
+        <v>61192</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
+        <v>61193</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
+        <v>61194</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A63" s="9">
+        <v>61195</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A64" s="9">
+        <v>61196</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
+        <v>61198</v>
+      </c>
+      <c r="B65" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6569509-97C1-4C00-933A-2630948AFC33}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="67" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="128.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>62071</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>61190</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>61525</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="C65" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
+        <v>61199</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
         <v>61201</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="B67" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="9">
+        <v>62030</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D68" s="10"/>
+      <c r="E68" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="9">
+        <v>64308</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70" s="11">
+        <v>61995</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="14">
+        <v>61997</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A72" s="14">
+        <v>65506</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A73" s="14">
+        <v>65507</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A74" s="14">
+        <v>65508</v>
+      </c>
+      <c r="B74" s="14" t="s">
         <v>16</v>
       </c>
-    </row>
+      <c r="C74" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="F74" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A75" s="14">
+        <v>62062</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E76" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
algunos cambios en los TC de credito Forzado
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDITO FORZADO- Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDITO FORZADO- Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FC5E09-E066-43DB-8524-60AA89562ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237D044E-DB63-4A80-88EA-A6EAE906FC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="158">
   <si>
     <t>Parametros</t>
   </si>
@@ -368,9 +368,6 @@
     <t>"operacion":{"vendedor":{"cuit":"20000001210","cbu":"9980000400000000000062","recurrencia":true,"prestacion":"Prestacion7"},"comprador":{"cuit":"20000001210","cuenta":{"cbu":"9980000400000000000246"}},"detalle":{"importe":199.02}}}|"operacion":{"comprador":{"cuit":"20000001210","cuenta":{"cbu":"9980000400000000000246"}},"detalle":{"importe":199.02}}}|"id":"debin.id","aviso":"all","endpoint":"Codigo03","producto":"responder"</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001210","cbu":"9980000400000000000079","recurrencia":true,"prestacion":"Prestacion8"},"comprador":{"cuit":"20000001210","cuenta":{"cbu":"9980000400000000000253"}},"detalle":{"importe":199.02}}}|"operacion":{"comprador":{"cuit":"20000001210","cuenta":{"cbu":"9980000400000000000253"}},"detalle":{"importe":199.02}}}|"id":"debin.id","aviso":"all","endpoint":"Codigo04","producto":"responder"</t>
-  </si>
-  <si>
     <t>"operacion":{"vendedor":{"cuit":"20000001210","cbu":"9980000400000000000086","recurrencia":true,"prestacion":"Prestacion9"},"comprador":{"cuit":"20000001210","cuenta":{"cbu":"9980000400000000000260"}},"detalle":{"importe":199.02}}}|"operacion":{"comprador":{"cuit":"20000001210","cuenta":{"cbu":"9980000400000000000260"}},"detalle":{"importe":199.02}}}|"id":"debin.id","aviso":"all","endpoint":"Codigo06","producto":"responder"</t>
   </si>
   <si>
@@ -407,9 +404,6 @@
     <t>"operacion":{"vendedor":{"cuit":"20000001563","cbu":"0000479800000000000000","banco":"000","recurrencia":true},"comprador":{"cuit":"20000001563","cuenta":{"cbu":"0000479800000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001563","cuenta":{"cbu":"0000479800000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001563","cuenta":{"cbu":"9980000400000000000529"}}}}|"id":"debin.id","aviso":"all","endpoint":"SpotCVU02","producto":"responder"</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001598","cbu":"0000483500000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion1"},"comprador":{"cuit":"20000001598","cuenta":{"cbu":"0000483500000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001598","cuenta":{"cbu":"0000483500000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001598","cuenta":{"cbu":"9980000400000000000574"}}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
     <t>"operacion":{"vendedor":{"cuit":"20000001601","cbu":"0000485900000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion2"},"comprador":{"cuit":"20000001601","cuenta":{"cbu":"0000485900000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001601","cuenta":{"cbu":"0000485900000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001601","cuenta":{"cbu":"9980000400000000000598"}}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
   </si>
   <si>
@@ -461,9 +455,6 @@
     <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 03: Cuenta inexistente - Debin QR Coelsa Coelsa</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001776","cbu":"'0000476700000000000000","banco":"000","sucursal":"0476"},"comprador":{"cuenta":{"cbu":"0000476700000000000017"},"cuit":"20000001776"},"detalle":{"importe":1000,"id_billetera":476}}}|"operacion":{"comprador":{"cuit":"20000001776","cuenta":{"cbu":"9980000400000000000895"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
     <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 04: Cuenta no habilitada - Debin QR Coelsa Coelsa</t>
   </si>
   <si>
@@ -479,9 +470,6 @@
     <t xml:space="preserve">Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 02: Datos incorrectos - Debin QR Coelsa Coelsa - OK </t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001784","cbu":"0000474300000000000000","banco":"000","sucursal":"0474"},"comprador":{"cuenta":{"cbu":"0000126300000000000017"},"cuit":"20000001784"},"detalle":{"importe":1000,"id_billetera":474}}}|"operacion":{"comprador":{"cuit":"20000001784","cuenta":{"cbu":"9980000400000000000918"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 05: Error interno - Debin QR Coelsa Coelsa - OK </t>
   </si>
   <si>
@@ -491,9 +479,6 @@
     <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 403 - Contracargo QR Coelsa Coelsa - OK</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001725","cbu":"0000484200000000000000","banco":"000","sucursal":"0484"},"comprador":{"cuenta":{"cbu":"0000484200000000000017"},"cuit":"20000001725"},"detalle":{"importe":1000,"id_billetera":484}}}|"operacion":{"comprador":{"cuit":"20000001725","cuenta":{"cbu":"9980000400000000000819"}},"detalle":{"importe":1000}}}|"operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20000001725","cbu":"0000484200000000000000"}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
     <t>Credito Forzado - Agregado a broker/push - AvisoCredito responde 404 - Contracargo QR Coelsa Coelsa - OK</t>
   </si>
   <si>
@@ -503,16 +488,28 @@
     <t>Crédito Forzado - Agregado a broker/push - AvisoCredito responde un 200 con código 00: Crédito realizado - Contracargo QR Coelsa Coelsa - OK</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001725","cbu":"0000484200000000000000","banco":"000","sucursal":"0484"},"comprador":{"cuenta":{"cbu":"0000484200000000000017"},"cuit":"20000001725"},"detalle":{"importe":10,"id_billetera":484}}}|"operacion":{"comprador":{"cuit":"20000001725","cuenta":{"cbu":"9980000400000000000819"}},"detalle":{"importe":10}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
-  </si>
-  <si>
     <t>"operacion":{"vendedor":{"cuit":"20000001717","cbu":"0000486600000000000000","banco":"000","sucursal":"0486"},"comprador":{"cuenta":{"cbu":"0000486600000000000017"},"cuit":"20000001717"},"detalle":{"importe":10,"id_billetera":486}}}|"operacion":{"comprador":{"cuit":"20000001717","cuenta":{"cbu":"9980000400000000000796"}},"detalle":{"importe":10}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
   </si>
   <si>
-    <t>"operacion":{"vendedor":{"cuit":"20000001652","cbu":"0000494100000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion6"},"comprador":{"cuit":"20000001652","cuenta":{"cbu":"0000494100000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001652","cuenta":{"cbu":"0000494100000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001652","cuenta":{"cbu":"9980000400000000000673"}}}}|"id":"debin.id","aviso":"all","endpoint":"RecCVU04","producto":"responder"</t>
-  </si>
-  <si>
     <t>"operacion":{"vendedor":{"cuit":"20000001555","cbu":"0000495800000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion7"},"comprador":{"cuit":"20000001555","cuenta":{"cbu":"0000495800000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001555","cuenta":{"cbu":"0000495800000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001660","cuenta":{"cbu":"9980000400000000000697"}}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001725","cbu":"0000484200000000000000","banco":"000","sucursal":"0484"},"comprador":{"cuenta":{"cbu":"0000484200000000000017"},"cuit":"20000001725"},"detalle":{"importe":10,"id_billetera":484}}}|"operacion":{"comprador":{"cuit":"20000001725","cuenta":{"cbu":"9980000400000000000802"}},"detalle":{"importe":10}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001725","cbu":"0000484200000000000000","banco":"000","sucursal":"0484"},"comprador":{"cuenta":{"cbu":"0000484200000000000017"},"cuit":"20000001725"},"detalle":{"importe":1000,"id_billetera":484}}}|"operacion":{"comprador":{"cuit":"20000001725","cuenta":{"cbu":"9980000400000000000802"}},"detalle":{"importe":1000}}}|"operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20000001725","cbu":"0000484200000000000000"}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001784","cbu":"0000474300000000000000","banco":"000","sucursal":"0474"},"comprador":{"cuenta":{"cbu":"0000474300000000000017"},"cuit":"20000001784"},"detalle":{"importe":1000,"id_billetera":474}}}|"operacion":{"comprador":{"cuit":"20000001784","cuenta":{"cbu":"9980000400000000000918"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001695","cbu":"0000489700000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion10"},"comprador":{"cuit":"20000001695","cuenta":{"cbu":"0000489700000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001695","cuenta":{"cbu":"0000489700000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001695","cuenta":{"cbu":"9980000400000000000758"}}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001652","cbu":"0000494100000000000000","banco":"000","recurrencia":true,"prestacion":"Prestacion6"},"comprador":{"cuit":"20000001652","cuenta":{"cbu":"0000494100000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001652","cuenta":{"cbu":"0000494100000000000017"}}}}|"operacion":{"comprador":{"cuit":"20000001652","cuenta":{"cbu":"9980000400000000000673"}}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"vendedor":{"cuit":"20000001776","cbu":"0000476700000000000000","banco":"000","sucursal":"0476"},"comprador":{"cuenta":{"cbu":"0000476700000000000017"},"cuit":"20000001776"},"detalle":{"importe":1000,"id_billetera":476}}}|"operacion":{"comprador":{"cuit":"20000001776","cuenta":{"cbu":"9980000400000000000895"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
   </si>
 </sst>
 </file>
@@ -867,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC0A671-2C0C-430F-865C-9634A4BA3E48}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,7 +1094,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>21</v>
@@ -1140,7 +1137,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>23</v>
@@ -1309,7 +1306,7 @@
         <v>9</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>48</v>
@@ -1323,7 +1320,7 @@
         <v>9</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>49</v>
@@ -1337,7 +1334,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>50</v>
@@ -1351,7 +1348,7 @@
         <v>9</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>51</v>
@@ -1365,7 +1362,7 @@
         <v>9</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>52</v>
@@ -1379,7 +1376,7 @@
         <v>9</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>53</v>
@@ -1393,7 +1390,7 @@
         <v>9</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>54</v>
@@ -1407,7 +1404,7 @@
         <v>9</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>55</v>
@@ -1421,7 +1418,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>56</v>
@@ -1547,7 +1544,7 @@
         <v>16</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>42</v>
@@ -1561,7 +1558,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9" t="s">
@@ -1576,7 +1573,7 @@
         <v>9</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9" t="s">
@@ -1591,7 +1588,7 @@
         <v>9</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9" t="s">
@@ -1606,7 +1603,7 @@
         <v>9</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9" t="s">
@@ -1621,14 +1618,14 @@
         <v>9</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>61171</v>
       </c>
@@ -1636,7 +1633,7 @@
         <v>9</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9" t="s">
@@ -1651,7 +1648,7 @@
         <v>9</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9" t="s">
@@ -1666,7 +1663,7 @@
         <v>9</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9" t="s">
@@ -1681,7 +1678,7 @@
         <v>9</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9" t="s">
@@ -1696,7 +1693,7 @@
         <v>11</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9" t="s">
@@ -1711,7 +1708,7 @@
         <v>11</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9" t="s">
@@ -1726,7 +1723,7 @@
         <v>11</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9" t="s">
@@ -1741,11 +1738,11 @@
         <v>10</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1756,11 +1753,11 @@
         <v>10</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1771,11 +1768,11 @@
         <v>10</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1786,11 +1783,11 @@
         <v>10</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1801,11 +1798,11 @@
         <v>10</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1816,11 +1813,11 @@
         <v>10</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1831,11 +1828,11 @@
         <v>10</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1846,11 +1843,11 @@
         <v>10</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1861,11 +1858,11 @@
         <v>10</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1876,11 +1873,11 @@
         <v>13</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1891,11 +1888,11 @@
         <v>13</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1906,11 +1903,11 @@
         <v>13</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Casos Debin QR (TRX3.0)
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - CREDITO FORZADO- Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - CREDITO FORZADO- Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107D84FE-450C-4E8B-AB31-052A1593246A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99244DC1-73AB-4886-9AC3-2177BCDF5918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="169">
   <si>
     <t>Parametros</t>
   </si>
@@ -535,6 +535,12 @@
   </si>
   <si>
     <t>"banco":"044","operacion":{"vendedor":{"cuit":"20000001059","cbu":"0000236500000000000000","banco":"000","sucursal":"0236"},"comprador":{"cuenta":{"cbu":"0000236500000000000017"},"cuit":"20000001059"},"detalle":{"importe":1000,"id_billetera":236}}}|"banco":"044","operacion":{"comprador":{"cuit":"20000000869","cuenta":{"cbu":"0440000400000000000895"}},"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"all","producto":"responder"</t>
+  </si>
+  <si>
+    <t>Contracargo Debin Recurrente - Modificación Control Garantías - Llamada Crédito/Débito - Caso OK</t>
+  </si>
+  <si>
+    <t>Contracargo Debin Recurrente - Modificación Control Garantías - Avisos con codigos correctos - ERROR 0120 en Garantias -&gt; 0510 FONDOS INSUF.</t>
   </si>
 </sst>
 </file>
@@ -630,7 +636,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -906,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC0A671-2C0C-430F-865C-9634A4BA3E48}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,6 +2141,34 @@
         <v>154</v>
       </c>
     </row>
+    <row r="82" spans="1:6" s="13" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A82" s="13">
+        <v>62309</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="13" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A83" s="13">
+        <v>62312</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>